<commit_message>
Added IoT examples. Reorganized example source. Built new package.
</commit_message>
<xml_diff>
--- a/source/_docs/Error Codes - AWS Toolkit - IAM.xlsx
+++ b/source/_docs/Error Codes - AWS Toolkit - IAM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Code</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>LimitExceeded - The request was rejected because it attempted to create resources beyond the current AWS account limits.</t>
+  </si>
+  <si>
+    <t>EntityAlreadyExists - The request was rejected because it attempted to create a resource that already exists.</t>
   </si>
 </sst>
 </file>
@@ -399,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -427,6 +430,14 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>412501</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>